<commit_message>
Remove elements of careteam end search param that are auto-added by IG Publisher e3a36a8da2b15bed6d4d879b0a1e3c24d0ac88f7
</commit_message>
<xml_diff>
--- a/ig/fix/#2-errors-gofsh/StructureDefinition-cds-bundle-transaction-creation.xlsx
+++ b/ig/fix/#2-errors-gofsh/StructureDefinition-cds-bundle-transaction-creation.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-06-26T08:37:35+00:00</t>
+    <t>2023-06-30T14:17:51+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2731,10 +2731,10 @@
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="S7" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="S7" t="s" s="2">
-        <v>34</v>
       </c>
       <c r="T7" t="s" s="2">
         <v>34</v>

</xml_diff>